<commit_message>
modified:   dsyg_erp/WebRoot/page/warehouserpt/updwarehouserptout.jsp 	modified:   dsyg_erp/WebRoot/page/warehouserpt_out_detail_inter_template.xlsx 	modified:   dsyg_erp/WebRoot/page/warehouserpt_out_detail_noprice_template.xlsx 	modified:   dsyg_erp/src/com/cn/common/factory/PoiWarehouserptOutDetail2.java 	modified:   dsyg_erp/src/com/cn/dsyg/action/WarehouserptAction.java 	modified:   dsyg_erp/src/com/cn/dsyg/service/impl/WarehouserptServiceImpl.java
</commit_message>
<xml_diff>
--- a/dsyg_erp/WebRoot/page/warehouserpt_out_detail_inter_template.xlsx
+++ b/dsyg_erp/WebRoot/page/warehouserpt_out_detail_inter_template.xlsx
@@ -251,7 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -287,14 +287,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="20"/>
       <color indexed="8"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -311,13 +303,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -365,6 +350,26 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -467,7 +472,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -475,9 +480,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -487,38 +489,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -527,18 +524,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,9 +854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -864,141 +873,141 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="26.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
     </row>
     <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="19" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="22"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="18"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="31"/>
     </row>
     <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="17"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="14"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="14"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="11"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="23" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="13"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="10"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
@@ -1007,50 +1016,50 @@
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="26" t="s">
+      <c r="C14" s="25"/>
+      <c r="D14" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="29"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="26" t="s">
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="26" t="s">
+      <c r="K14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="26" t="s">
+      <c r="L14" s="22" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>